<commit_message>
Final Commit with phone number validation and account exists verification
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://avaalisolutions-my.sharepoint.com/personal/sameer_shariff_avaali_com/Documents/Documents/UiPath/SalesAccountAutomation/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F26A15F7-DCEC-4DC1-A8C7-2AEBC4C52CCD}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3DACB8E-655E-435D-A6E9-77C0A35DEE41}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -589,7 +589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1727,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1778,7 +1778,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>25</v>

</xml_diff>